<commit_message>
Back to correct version
</commit_message>
<xml_diff>
--- a/MAST/data/ColeParker/Cole parker.xlsx
+++ b/MAST/data/ColeParker/Cole parker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhaoguowang/Documents/Developer/WorkSpace/Julia/playground/JuMP-Example/MAST/data/ColeParker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9034DE02-5FEE-A44E-84EE-B65FC9AC14C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335A5449-F1E4-AF4A-B86E-F2EDF26DB439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="5260" windowWidth="29140" windowHeight="12200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12360" yWindow="4840" windowWidth="29140" windowHeight="12200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generator Data" sheetId="1" r:id="rId1"/>
@@ -4688,8 +4688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -36308,7 +36308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>